<commit_message>
changed parameter estimation report to work with copasi version19 and modified parameter estimation to use it and give it proper titles
</commit_message>
<xml_diff>
--- a/PyCoTools/Tests/PEConfigFile.xlsx
+++ b/PyCoTools/Tests/PEConfigFile.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="54">
   <si>
     <t>start_value</t>
   </si>
@@ -79,13 +79,16 @@
     <t>F</t>
   </si>
   <si>
+    <t>10</t>
+  </si>
+  <si>
     <t>0.1</t>
   </si>
   <si>
-    <t>1.999999999999998</t>
-  </si>
-  <si>
-    <t>50</t>
+    <t>1.999999999999999</t>
+  </si>
+  <si>
+    <t>15</t>
   </si>
   <si>
     <t>1</t>
@@ -97,7 +100,7 @@
     <t>99.9999845072</t>
   </si>
   <si>
-    <t>9.99999845072</t>
+    <t>5.0</t>
   </si>
   <si>
     <t>9999.99845072</t>
@@ -567,19 +570,19 @@
         <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -587,22 +590,22 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -610,22 +613,22 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -633,22 +636,22 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -656,22 +659,22 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -679,22 +682,22 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -702,22 +705,22 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -725,22 +728,22 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -748,22 +751,22 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -771,22 +774,22 @@
         <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G11" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -794,22 +797,22 @@
         <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E12" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G12" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -817,22 +820,22 @@
         <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E13" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F13" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G13" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -840,22 +843,22 @@
         <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F14" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -863,22 +866,22 @@
         <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E15" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F15" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G15" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>